<commit_message>
updated outputs, and classify_meta
</commit_message>
<xml_diff>
--- a/outputs/p__Bacteroidota.xlsx
+++ b/outputs/p__Bacteroidota.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15880" tabRatio="600" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15880" tabRatio="600" firstSheet="9" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="g__Prevotella-t" sheetId="1" state="visible" r:id="rId1"/>
@@ -31,13 +31,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -57,12 +63,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -91,12 +112,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -6041,7 +6065,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="B1" s="2" t="inlineStr">
@@ -30662,7 +30686,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="B1" s="2" t="inlineStr">
@@ -31307,7 +31331,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="B1" s="2" t="inlineStr">
@@ -35786,7 +35810,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="B1" s="2" t="inlineStr">
@@ -41587,7 +41611,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="B1" s="2" t="inlineStr">
@@ -46897,7 +46921,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I196"/>
+  <dimension ref="A1:J196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -46906,49 +46930,54 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>c__Bacteroidia</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>c__Chlorobia</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>c__Ignavibacteria</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>c__Rhodothermia</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>c__UBA10030</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>max</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>prediction</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
+      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>rejection-f</t>
         </is>
       </c>
+      <c r="J1" s="3" t="inlineStr">
+        <is>
+          <t>gtdb-Tk</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>RUG152</t>
         </is>
@@ -46981,9 +47010,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>RUG419</t>
         </is>
@@ -47016,9 +47050,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
+      <c r="A4" s="3" t="inlineStr">
         <is>
           <t>hRUG908</t>
         </is>
@@ -47051,9 +47090,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="inlineStr">
+      <c r="A5" s="3" t="inlineStr">
         <is>
           <t>RUG459</t>
         </is>
@@ -47086,9 +47130,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="inlineStr">
+      <c r="A6" s="3" t="inlineStr">
         <is>
           <t>RUG577</t>
         </is>
@@ -47121,9 +47170,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="inlineStr">
+      <c r="A7" s="3" t="inlineStr">
         <is>
           <t>RUG431</t>
         </is>
@@ -47156,9 +47210,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="inlineStr">
+      <c r="A8" s="3" t="inlineStr">
         <is>
           <t>RUG446</t>
         </is>
@@ -47191,9 +47250,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="inlineStr">
+      <c r="A9" s="3" t="inlineStr">
         <is>
           <t>RUG318</t>
         </is>
@@ -47226,9 +47290,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="inlineStr">
+      <c r="A10" s="3" t="inlineStr">
         <is>
           <t>RUG483</t>
         </is>
@@ -47261,9 +47330,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="inlineStr">
+      <c r="A11" s="3" t="inlineStr">
         <is>
           <t>RUG326</t>
         </is>
@@ -47296,9 +47370,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="inlineStr">
+      <c r="A12" s="3" t="inlineStr">
         <is>
           <t>hRUG906</t>
         </is>
@@ -47331,9 +47410,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="inlineStr">
+      <c r="A13" s="3" t="inlineStr">
         <is>
           <t>RUG354</t>
         </is>
@@ -47366,9 +47450,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="inlineStr">
+      <c r="A14" s="3" t="inlineStr">
         <is>
           <t>RUG339</t>
         </is>
@@ -47401,9 +47490,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="inlineStr">
+      <c r="A15" s="3" t="inlineStr">
         <is>
           <t>RUG417</t>
         </is>
@@ -47436,9 +47530,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="inlineStr">
+      <c r="A16" s="3" t="inlineStr">
         <is>
           <t>RUG462</t>
         </is>
@@ -47471,9 +47570,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="2" t="inlineStr">
+      <c r="A17" s="3" t="inlineStr">
         <is>
           <t>RUG362</t>
         </is>
@@ -47506,9 +47610,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="2" t="inlineStr">
+      <c r="A18" s="3" t="inlineStr">
         <is>
           <t>RUG500</t>
         </is>
@@ -47541,9 +47650,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="2" t="inlineStr">
+      <c r="A19" s="3" t="inlineStr">
         <is>
           <t>RUG273</t>
         </is>
@@ -47576,9 +47690,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" s="2" t="inlineStr">
+      <c r="A20" s="3" t="inlineStr">
         <is>
           <t>RUG307</t>
         </is>
@@ -47611,9 +47730,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" s="2" t="inlineStr">
+      <c r="A21" s="3" t="inlineStr">
         <is>
           <t>RUG397</t>
         </is>
@@ -47646,9 +47770,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" s="2" t="inlineStr">
+      <c r="A22" s="3" t="inlineStr">
         <is>
           <t>RUG569</t>
         </is>
@@ -47681,9 +47810,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" s="2" t="inlineStr">
+      <c r="A23" s="3" t="inlineStr">
         <is>
           <t>RUG474</t>
         </is>
@@ -47716,9 +47850,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" s="2" t="inlineStr">
+      <c r="A24" s="3" t="inlineStr">
         <is>
           <t>hRUG897</t>
         </is>
@@ -47751,9 +47890,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" s="2" t="inlineStr">
+      <c r="A25" s="3" t="inlineStr">
         <is>
           <t>RUG323</t>
         </is>
@@ -47786,9 +47930,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" s="2" t="inlineStr">
+      <c r="A26" s="3" t="inlineStr">
         <is>
           <t>RUG367</t>
         </is>
@@ -47821,9 +47970,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" s="2" t="inlineStr">
+      <c r="A27" s="3" t="inlineStr">
         <is>
           <t>RUG538</t>
         </is>
@@ -47856,9 +48010,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" s="2" t="inlineStr">
+      <c r="A28" s="3" t="inlineStr">
         <is>
           <t>RUG153</t>
         </is>
@@ -47891,9 +48050,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" s="2" t="inlineStr">
+      <c r="A29" s="3" t="inlineStr">
         <is>
           <t>RUG429</t>
         </is>
@@ -47926,9 +48090,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" s="2" t="inlineStr">
+      <c r="A30" s="3" t="inlineStr">
         <is>
           <t>RUG144</t>
         </is>
@@ -47961,9 +48130,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" s="2" t="inlineStr">
+      <c r="A31" s="3" t="inlineStr">
         <is>
           <t>RUG423</t>
         </is>
@@ -47996,9 +48170,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" s="2" t="inlineStr">
+      <c r="A32" s="3" t="inlineStr">
         <is>
           <t>RUG407</t>
         </is>
@@ -48031,9 +48210,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" s="2" t="inlineStr">
+      <c r="A33" s="3" t="inlineStr">
         <is>
           <t>hRUG858</t>
         </is>
@@ -48066,9 +48250,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="34">
-      <c r="A34" s="2" t="inlineStr">
+      <c r="A34" s="3" t="inlineStr">
         <is>
           <t>RUG168</t>
         </is>
@@ -48101,9 +48290,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" s="2" t="inlineStr">
+      <c r="A35" s="3" t="inlineStr">
         <is>
           <t>RUG242</t>
         </is>
@@ -48136,9 +48330,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" s="2" t="inlineStr">
+      <c r="A36" s="3" t="inlineStr">
         <is>
           <t>RUG106</t>
         </is>
@@ -48171,9 +48370,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="37">
-      <c r="A37" s="2" t="inlineStr">
+      <c r="A37" s="3" t="inlineStr">
         <is>
           <t>RUG259</t>
         </is>
@@ -48206,9 +48410,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" s="2" t="inlineStr">
+      <c r="A38" s="3" t="inlineStr">
         <is>
           <t>RUG739</t>
         </is>
@@ -48241,9 +48450,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="39">
-      <c r="A39" s="2" t="inlineStr">
+      <c r="A39" s="3" t="inlineStr">
         <is>
           <t>RUG559</t>
         </is>
@@ -48276,9 +48490,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="40">
-      <c r="A40" s="2" t="inlineStr">
+      <c r="A40" s="3" t="inlineStr">
         <is>
           <t>RUG488</t>
         </is>
@@ -48311,9 +48530,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="41">
-      <c r="A41" s="2" t="inlineStr">
+      <c r="A41" s="3" t="inlineStr">
         <is>
           <t>RUG085</t>
         </is>
@@ -48346,9 +48570,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="42">
-      <c r="A42" s="2" t="inlineStr">
+      <c r="A42" s="3" t="inlineStr">
         <is>
           <t>RUG156</t>
         </is>
@@ -48381,9 +48610,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="43">
-      <c r="A43" s="2" t="inlineStr">
+      <c r="A43" s="3" t="inlineStr">
         <is>
           <t>RUG647</t>
         </is>
@@ -48416,9 +48650,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="44">
-      <c r="A44" s="2" t="inlineStr">
+      <c r="A44" s="3" t="inlineStr">
         <is>
           <t>RUG733</t>
         </is>
@@ -48451,9 +48690,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="45">
-      <c r="A45" s="2" t="inlineStr">
+      <c r="A45" s="3" t="inlineStr">
         <is>
           <t>RUG064</t>
         </is>
@@ -48486,9 +48730,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="46">
-      <c r="A46" s="2" t="inlineStr">
+      <c r="A46" s="3" t="inlineStr">
         <is>
           <t>RUG849</t>
         </is>
@@ -48521,9 +48770,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="47">
-      <c r="A47" s="2" t="inlineStr">
+      <c r="A47" s="3" t="inlineStr">
         <is>
           <t>RUG216</t>
         </is>
@@ -48556,9 +48810,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="48">
-      <c r="A48" s="2" t="inlineStr">
+      <c r="A48" s="3" t="inlineStr">
         <is>
           <t>hRUG893</t>
         </is>
@@ -48591,9 +48850,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="49">
-      <c r="A49" s="2" t="inlineStr">
+      <c r="A49" s="3" t="inlineStr">
         <is>
           <t>RUG200</t>
         </is>
@@ -48626,9 +48890,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="50">
-      <c r="A50" s="2" t="inlineStr">
+      <c r="A50" s="3" t="inlineStr">
         <is>
           <t>RUG083</t>
         </is>
@@ -48661,9 +48930,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="51">
-      <c r="A51" s="2" t="inlineStr">
+      <c r="A51" s="3" t="inlineStr">
         <is>
           <t>RUG309</t>
         </is>
@@ -48696,9 +48970,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="52">
-      <c r="A52" s="2" t="inlineStr">
+      <c r="A52" s="3" t="inlineStr">
         <is>
           <t>RUG550</t>
         </is>
@@ -48731,9 +49010,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="53">
-      <c r="A53" s="2" t="inlineStr">
+      <c r="A53" s="3" t="inlineStr">
         <is>
           <t>RUG360</t>
         </is>
@@ -48766,9 +49050,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="54">
-      <c r="A54" s="2" t="inlineStr">
+      <c r="A54" s="3" t="inlineStr">
         <is>
           <t>RUG782</t>
         </is>
@@ -48801,9 +49090,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="55">
-      <c r="A55" s="2" t="inlineStr">
+      <c r="A55" s="3" t="inlineStr">
         <is>
           <t>RUG003</t>
         </is>
@@ -48836,9 +49130,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="56">
-      <c r="A56" s="2" t="inlineStr">
+      <c r="A56" s="3" t="inlineStr">
         <is>
           <t>RUG575</t>
         </is>
@@ -48871,9 +49170,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="57">
-      <c r="A57" s="2" t="inlineStr">
+      <c r="A57" s="3" t="inlineStr">
         <is>
           <t>RUG535</t>
         </is>
@@ -48906,9 +49210,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="58">
-      <c r="A58" s="2" t="inlineStr">
+      <c r="A58" s="3" t="inlineStr">
         <is>
           <t>RUG315</t>
         </is>
@@ -48941,9 +49250,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="59">
-      <c r="A59" s="2" t="inlineStr">
+      <c r="A59" s="3" t="inlineStr">
         <is>
           <t>RUG392</t>
         </is>
@@ -48976,9 +49290,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="60">
-      <c r="A60" s="2" t="inlineStr">
+      <c r="A60" s="3" t="inlineStr">
         <is>
           <t>RUG108</t>
         </is>
@@ -49011,9 +49330,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="61">
-      <c r="A61" s="2" t="inlineStr">
+      <c r="A61" s="3" t="inlineStr">
         <is>
           <t>RUG541</t>
         </is>
@@ -49046,9 +49370,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="62">
-      <c r="A62" s="2" t="inlineStr">
+      <c r="A62" s="3" t="inlineStr">
         <is>
           <t>RUG461</t>
         </is>
@@ -49081,9 +49410,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="63">
-      <c r="A63" s="2" t="inlineStr">
+      <c r="A63" s="3" t="inlineStr">
         <is>
           <t>RUG378</t>
         </is>
@@ -49116,9 +49450,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="64">
-      <c r="A64" s="2" t="inlineStr">
+      <c r="A64" s="3" t="inlineStr">
         <is>
           <t>RUG250</t>
         </is>
@@ -49151,9 +49490,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="65">
-      <c r="A65" s="2" t="inlineStr">
+      <c r="A65" s="3" t="inlineStr">
         <is>
           <t>RUG546</t>
         </is>
@@ -49186,9 +49530,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="66">
-      <c r="A66" s="2" t="inlineStr">
+      <c r="A66" s="3" t="inlineStr">
         <is>
           <t>RUG195</t>
         </is>
@@ -49221,9 +49570,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="67">
-      <c r="A67" s="2" t="inlineStr">
+      <c r="A67" s="3" t="inlineStr">
         <is>
           <t>RUG660</t>
         </is>
@@ -49256,9 +49610,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="68">
-      <c r="A68" s="2" t="inlineStr">
+      <c r="A68" s="3" t="inlineStr">
         <is>
           <t>RUG734</t>
         </is>
@@ -49291,9 +49650,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="69">
-      <c r="A69" s="2" t="inlineStr">
+      <c r="A69" s="3" t="inlineStr">
         <is>
           <t>RUG061</t>
         </is>
@@ -49326,9 +49690,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="70">
-      <c r="A70" s="2" t="inlineStr">
+      <c r="A70" s="3" t="inlineStr">
         <is>
           <t>RUG280</t>
         </is>
@@ -49361,9 +49730,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="71">
-      <c r="A71" s="2" t="inlineStr">
+      <c r="A71" s="3" t="inlineStr">
         <is>
           <t>RUG548</t>
         </is>
@@ -49396,9 +49770,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="72">
-      <c r="A72" s="2" t="inlineStr">
+      <c r="A72" s="3" t="inlineStr">
         <is>
           <t>hRUG888</t>
         </is>
@@ -49431,9 +49810,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="73">
-      <c r="A73" s="2" t="inlineStr">
+      <c r="A73" s="3" t="inlineStr">
         <is>
           <t>RUG614</t>
         </is>
@@ -49466,9 +49850,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="74">
-      <c r="A74" s="2" t="inlineStr">
+      <c r="A74" s="3" t="inlineStr">
         <is>
           <t>RUG278</t>
         </is>
@@ -49501,9 +49890,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="75">
-      <c r="A75" s="2" t="inlineStr">
+      <c r="A75" s="3" t="inlineStr">
         <is>
           <t>RUG755</t>
         </is>
@@ -49536,9 +49930,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="76">
-      <c r="A76" s="2" t="inlineStr">
+      <c r="A76" s="3" t="inlineStr">
         <is>
           <t>RUG539</t>
         </is>
@@ -49571,9 +49970,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="77">
-      <c r="A77" s="2" t="inlineStr">
+      <c r="A77" s="3" t="inlineStr">
         <is>
           <t>RUG676</t>
         </is>
@@ -49606,9 +50010,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="78">
-      <c r="A78" s="2" t="inlineStr">
+      <c r="A78" s="3" t="inlineStr">
         <is>
           <t>RUG742</t>
         </is>
@@ -49641,9 +50050,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="79">
-      <c r="A79" s="2" t="inlineStr">
+      <c r="A79" s="3" t="inlineStr">
         <is>
           <t>RUG723</t>
         </is>
@@ -49676,9 +50090,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="80">
-      <c r="A80" s="2" t="inlineStr">
+      <c r="A80" s="3" t="inlineStr">
         <is>
           <t>RUG197</t>
         </is>
@@ -49711,9 +50130,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="81">
-      <c r="A81" s="2" t="inlineStr">
+      <c r="A81" s="3" t="inlineStr">
         <is>
           <t>RUG046</t>
         </is>
@@ -49746,9 +50170,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="82">
-      <c r="A82" s="2" t="inlineStr">
+      <c r="A82" s="3" t="inlineStr">
         <is>
           <t>RUG445</t>
         </is>
@@ -49781,9 +50210,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="83">
-      <c r="A83" s="2" t="inlineStr">
+      <c r="A83" s="3" t="inlineStr">
         <is>
           <t>RUG435</t>
         </is>
@@ -49816,9 +50250,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="84">
-      <c r="A84" s="2" t="inlineStr">
+      <c r="A84" s="3" t="inlineStr">
         <is>
           <t>RUG828</t>
         </is>
@@ -49851,9 +50290,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="85">
-      <c r="A85" s="2" t="inlineStr">
+      <c r="A85" s="3" t="inlineStr">
         <is>
           <t>RUG172</t>
         </is>
@@ -49886,9 +50330,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="86">
-      <c r="A86" s="2" t="inlineStr">
+      <c r="A86" s="3" t="inlineStr">
         <is>
           <t>RUG716</t>
         </is>
@@ -49921,9 +50370,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="87">
-      <c r="A87" s="2" t="inlineStr">
+      <c r="A87" s="3" t="inlineStr">
         <is>
           <t>RUG264</t>
         </is>
@@ -49956,9 +50410,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="88">
-      <c r="A88" s="2" t="inlineStr">
+      <c r="A88" s="3" t="inlineStr">
         <is>
           <t>RUG169</t>
         </is>
@@ -49991,9 +50450,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="89">
-      <c r="A89" s="2" t="inlineStr">
+      <c r="A89" s="3" t="inlineStr">
         <is>
           <t>RUG030</t>
         </is>
@@ -50026,9 +50490,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="90">
-      <c r="A90" s="2" t="inlineStr">
+      <c r="A90" s="3" t="inlineStr">
         <is>
           <t>RUG037</t>
         </is>
@@ -50061,9 +50530,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="91">
-      <c r="A91" s="2" t="inlineStr">
+      <c r="A91" s="3" t="inlineStr">
         <is>
           <t>RUG184</t>
         </is>
@@ -50096,9 +50570,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="92">
-      <c r="A92" s="2" t="inlineStr">
+      <c r="A92" s="3" t="inlineStr">
         <is>
           <t>RUG711</t>
         </is>
@@ -50131,9 +50610,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="93">
-      <c r="A93" s="2" t="inlineStr">
+      <c r="A93" s="3" t="inlineStr">
         <is>
           <t>RUG359</t>
         </is>
@@ -50166,9 +50650,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="94">
-      <c r="A94" s="2" t="inlineStr">
+      <c r="A94" s="3" t="inlineStr">
         <is>
           <t>RUG788</t>
         </is>
@@ -50201,9 +50690,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="95">
-      <c r="A95" s="2" t="inlineStr">
+      <c r="A95" s="3" t="inlineStr">
         <is>
           <t>RUG210</t>
         </is>
@@ -50236,9 +50730,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="96">
-      <c r="A96" s="2" t="inlineStr">
+      <c r="A96" s="3" t="inlineStr">
         <is>
           <t>RUG176</t>
         </is>
@@ -50271,9 +50770,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J96" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="97">
-      <c r="A97" s="2" t="inlineStr">
+      <c r="A97" s="3" t="inlineStr">
         <is>
           <t>RUG047</t>
         </is>
@@ -50306,9 +50810,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J97" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="98">
-      <c r="A98" s="2" t="inlineStr">
+      <c r="A98" s="3" t="inlineStr">
         <is>
           <t>RUG310</t>
         </is>
@@ -50341,9 +50850,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J98" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="99">
-      <c r="A99" s="2" t="inlineStr">
+      <c r="A99" s="3" t="inlineStr">
         <is>
           <t>RUG405</t>
         </is>
@@ -50376,9 +50890,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J99" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="100">
-      <c r="A100" s="2" t="inlineStr">
+      <c r="A100" s="3" t="inlineStr">
         <is>
           <t>hRUG883</t>
         </is>
@@ -50411,9 +50930,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J100" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="101">
-      <c r="A101" s="2" t="inlineStr">
+      <c r="A101" s="3" t="inlineStr">
         <is>
           <t>hRUG905</t>
         </is>
@@ -50446,9 +50970,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J101" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="102">
-      <c r="A102" s="2" t="inlineStr">
+      <c r="A102" s="3" t="inlineStr">
         <is>
           <t>RUG192</t>
         </is>
@@ -50481,9 +51010,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J102" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="103">
-      <c r="A103" s="2" t="inlineStr">
+      <c r="A103" s="3" t="inlineStr">
         <is>
           <t>RUG465</t>
         </is>
@@ -50516,9 +51050,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J103" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="104">
-      <c r="A104" s="2" t="inlineStr">
+      <c r="A104" s="3" t="inlineStr">
         <is>
           <t>RUG697</t>
         </is>
@@ -50551,9 +51090,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J104" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="105">
-      <c r="A105" s="2" t="inlineStr">
+      <c r="A105" s="3" t="inlineStr">
         <is>
           <t>RUG325</t>
         </is>
@@ -50586,9 +51130,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J105" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="106">
-      <c r="A106" s="2" t="inlineStr">
+      <c r="A106" s="3" t="inlineStr">
         <is>
           <t>RUG737</t>
         </is>
@@ -50621,9 +51170,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J106" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="107">
-      <c r="A107" s="2" t="inlineStr">
+      <c r="A107" s="3" t="inlineStr">
         <is>
           <t>RUG562</t>
         </is>
@@ -50656,9 +51210,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J107" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="108">
-      <c r="A108" s="2" t="inlineStr">
+      <c r="A108" s="3" t="inlineStr">
         <is>
           <t>RUG292</t>
         </is>
@@ -50691,9 +51250,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J108" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="109">
-      <c r="A109" s="2" t="inlineStr">
+      <c r="A109" s="3" t="inlineStr">
         <is>
           <t>RUG377</t>
         </is>
@@ -50726,9 +51290,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J109" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="110">
-      <c r="A110" s="2" t="inlineStr">
+      <c r="A110" s="3" t="inlineStr">
         <is>
           <t>RUG473</t>
         </is>
@@ -50761,9 +51330,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J110" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="111">
-      <c r="A111" s="2" t="inlineStr">
+      <c r="A111" s="3" t="inlineStr">
         <is>
           <t>RUG699</t>
         </is>
@@ -50796,9 +51370,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J111" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="112">
-      <c r="A112" s="2" t="inlineStr">
+      <c r="A112" s="3" t="inlineStr">
         <is>
           <t>RUG302</t>
         </is>
@@ -50831,9 +51410,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J112" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="113">
-      <c r="A113" s="2" t="inlineStr">
+      <c r="A113" s="3" t="inlineStr">
         <is>
           <t>RUG233</t>
         </is>
@@ -50866,9 +51450,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J113" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="114">
-      <c r="A114" s="2" t="inlineStr">
+      <c r="A114" s="3" t="inlineStr">
         <is>
           <t>RUG649</t>
         </is>
@@ -50901,9 +51490,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J114" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="115">
-      <c r="A115" s="2" t="inlineStr">
+      <c r="A115" s="3" t="inlineStr">
         <is>
           <t>RUG329</t>
         </is>
@@ -50936,9 +51530,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J115" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="116">
-      <c r="A116" s="2" t="inlineStr">
+      <c r="A116" s="3" t="inlineStr">
         <is>
           <t>RUG173</t>
         </is>
@@ -50971,9 +51570,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J116" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="117">
-      <c r="A117" s="2" t="inlineStr">
+      <c r="A117" s="3" t="inlineStr">
         <is>
           <t>RUG219</t>
         </is>
@@ -51006,9 +51610,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J117" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="118">
-      <c r="A118" s="2" t="inlineStr">
+      <c r="A118" s="3" t="inlineStr">
         <is>
           <t>RUG507</t>
         </is>
@@ -51041,9 +51650,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J118" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="119">
-      <c r="A119" s="2" t="inlineStr">
+      <c r="A119" s="3" t="inlineStr">
         <is>
           <t>RUG079</t>
         </is>
@@ -51076,9 +51690,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J119" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="120">
-      <c r="A120" s="2" t="inlineStr">
+      <c r="A120" s="3" t="inlineStr">
         <is>
           <t>RUG659</t>
         </is>
@@ -51111,9 +51730,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J120" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="121">
-      <c r="A121" s="2" t="inlineStr">
+      <c r="A121" s="3" t="inlineStr">
         <is>
           <t>RUG469</t>
         </is>
@@ -51146,9 +51770,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J121" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="122">
-      <c r="A122" s="2" t="inlineStr">
+      <c r="A122" s="3" t="inlineStr">
         <is>
           <t>RUG582</t>
         </is>
@@ -51181,9 +51810,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J122" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="123">
-      <c r="A123" s="2" t="inlineStr">
+      <c r="A123" s="3" t="inlineStr">
         <is>
           <t>RUG418</t>
         </is>
@@ -51216,9 +51850,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J123" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="124">
-      <c r="A124" s="2" t="inlineStr">
+      <c r="A124" s="3" t="inlineStr">
         <is>
           <t>RUG685</t>
         </is>
@@ -51251,9 +51890,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J124" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="125">
-      <c r="A125" s="2" t="inlineStr">
+      <c r="A125" s="3" t="inlineStr">
         <is>
           <t>RUG279</t>
         </is>
@@ -51286,9 +51930,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J125" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="126">
-      <c r="A126" s="2" t="inlineStr">
+      <c r="A126" s="3" t="inlineStr">
         <is>
           <t>RUG759</t>
         </is>
@@ -51321,9 +51970,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J126" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="127">
-      <c r="A127" s="2" t="inlineStr">
+      <c r="A127" s="3" t="inlineStr">
         <is>
           <t>RUG691</t>
         </is>
@@ -51356,9 +52010,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J127" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="128">
-      <c r="A128" s="2" t="inlineStr">
+      <c r="A128" s="3" t="inlineStr">
         <is>
           <t>RUG056</t>
         </is>
@@ -51391,9 +52050,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J128" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="129">
-      <c r="A129" s="2" t="inlineStr">
+      <c r="A129" s="3" t="inlineStr">
         <is>
           <t>RUG124</t>
         </is>
@@ -51426,9 +52090,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J129" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="130">
-      <c r="A130" s="2" t="inlineStr">
+      <c r="A130" s="3" t="inlineStr">
         <is>
           <t>RUG324</t>
         </is>
@@ -51461,9 +52130,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J130" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="131">
-      <c r="A131" s="2" t="inlineStr">
+      <c r="A131" s="3" t="inlineStr">
         <is>
           <t>RUG390</t>
         </is>
@@ -51496,9 +52170,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J131" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="132">
-      <c r="A132" s="2" t="inlineStr">
+      <c r="A132" s="3" t="inlineStr">
         <is>
           <t>RUG160</t>
         </is>
@@ -51531,9 +52210,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J132" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="133">
-      <c r="A133" s="2" t="inlineStr">
+      <c r="A133" s="3" t="inlineStr">
         <is>
           <t>RUG587</t>
         </is>
@@ -51566,9 +52250,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J133" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="134">
-      <c r="A134" s="2" t="inlineStr">
+      <c r="A134" s="3" t="inlineStr">
         <is>
           <t>RUG624</t>
         </is>
@@ -51601,9 +52290,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J134" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="135">
-      <c r="A135" s="2" t="inlineStr">
+      <c r="A135" s="3" t="inlineStr">
         <is>
           <t>RUG482</t>
         </is>
@@ -51636,9 +52330,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J135" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="136">
-      <c r="A136" s="2" t="inlineStr">
+      <c r="A136" s="3" t="inlineStr">
         <is>
           <t>RUG380</t>
         </is>
@@ -51671,9 +52370,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J136" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="137">
-      <c r="A137" s="2" t="inlineStr">
+      <c r="A137" s="3" t="inlineStr">
         <is>
           <t>RUG209</t>
         </is>
@@ -51706,9 +52410,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J137" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="138">
-      <c r="A138" s="2" t="inlineStr">
+      <c r="A138" s="3" t="inlineStr">
         <is>
           <t>RUG812</t>
         </is>
@@ -51741,9 +52450,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J138" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="139">
-      <c r="A139" s="2" t="inlineStr">
+      <c r="A139" s="3" t="inlineStr">
         <is>
           <t>RUG602</t>
         </is>
@@ -51776,9 +52490,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J139" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="140">
-      <c r="A140" s="2" t="inlineStr">
+      <c r="A140" s="3" t="inlineStr">
         <is>
           <t>RUG101</t>
         </is>
@@ -51811,9 +52530,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J140" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="141">
-      <c r="A141" s="2" t="inlineStr">
+      <c r="A141" s="3" t="inlineStr">
         <is>
           <t>RUG693</t>
         </is>
@@ -51846,9 +52570,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J141" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="142">
-      <c r="A142" s="2" t="inlineStr">
+      <c r="A142" s="3" t="inlineStr">
         <is>
           <t>RUG749</t>
         </is>
@@ -51881,9 +52610,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J142" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="143">
-      <c r="A143" s="2" t="inlineStr">
+      <c r="A143" s="3" t="inlineStr">
         <is>
           <t>RUG107</t>
         </is>
@@ -51916,9 +52650,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J143" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="144">
-      <c r="A144" s="2" t="inlineStr">
+      <c r="A144" s="3" t="inlineStr">
         <is>
           <t>RUG519</t>
         </is>
@@ -51951,9 +52690,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J144" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="145">
-      <c r="A145" s="2" t="inlineStr">
+      <c r="A145" s="3" t="inlineStr">
         <is>
           <t>RUG245</t>
         </is>
@@ -51986,9 +52730,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J145" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="146">
-      <c r="A146" s="2" t="inlineStr">
+      <c r="A146" s="3" t="inlineStr">
         <is>
           <t>RUG164</t>
         </is>
@@ -52021,9 +52770,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J146" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="147">
-      <c r="A147" s="2" t="inlineStr">
+      <c r="A147" s="3" t="inlineStr">
         <is>
           <t>RUG178</t>
         </is>
@@ -52056,9 +52810,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J147" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="148">
-      <c r="A148" s="2" t="inlineStr">
+      <c r="A148" s="3" t="inlineStr">
         <is>
           <t>RUG414</t>
         </is>
@@ -52091,9 +52850,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J148" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="149">
-      <c r="A149" s="2" t="inlineStr">
+      <c r="A149" s="3" t="inlineStr">
         <is>
           <t>RUG058</t>
         </is>
@@ -52126,9 +52890,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J149" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="150">
-      <c r="A150" s="2" t="inlineStr">
+      <c r="A150" s="3" t="inlineStr">
         <is>
           <t>RUG771</t>
         </is>
@@ -52161,9 +52930,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J150" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="151">
-      <c r="A151" s="2" t="inlineStr">
+      <c r="A151" s="3" t="inlineStr">
         <is>
           <t>RUG837</t>
         </is>
@@ -52196,9 +52970,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J151" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="152">
-      <c r="A152" s="2" t="inlineStr">
+      <c r="A152" s="3" t="inlineStr">
         <is>
           <t>RUG827</t>
         </is>
@@ -52231,9 +53010,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J152" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="153">
-      <c r="A153" s="2" t="inlineStr">
+      <c r="A153" s="3" t="inlineStr">
         <is>
           <t>hRUG857</t>
         </is>
@@ -52266,9 +53050,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J153" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="154">
-      <c r="A154" s="2" t="inlineStr">
+      <c r="A154" s="3" t="inlineStr">
         <is>
           <t>RUG843</t>
         </is>
@@ -52301,9 +53090,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J154" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="155">
-      <c r="A155" s="2" t="inlineStr">
+      <c r="A155" s="3" t="inlineStr">
         <is>
           <t>RUG689</t>
         </is>
@@ -52336,9 +53130,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J155" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="156">
-      <c r="A156" s="2" t="inlineStr">
+      <c r="A156" s="3" t="inlineStr">
         <is>
           <t>RUG165</t>
         </is>
@@ -52371,9 +53170,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J156" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="157">
-      <c r="A157" s="2" t="inlineStr">
+      <c r="A157" s="3" t="inlineStr">
         <is>
           <t>RUG451</t>
         </is>
@@ -52406,9 +53210,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J157" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="158">
-      <c r="A158" s="2" t="inlineStr">
+      <c r="A158" s="3" t="inlineStr">
         <is>
           <t>RUG536</t>
         </is>
@@ -52441,9 +53250,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J158" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="159">
-      <c r="A159" s="2" t="inlineStr">
+      <c r="A159" s="3" t="inlineStr">
         <is>
           <t>RUG506</t>
         </is>
@@ -52476,9 +53290,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J159" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="160">
-      <c r="A160" s="2" t="inlineStr">
+      <c r="A160" s="3" t="inlineStr">
         <is>
           <t>RUG606</t>
         </is>
@@ -52511,9 +53330,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J160" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="161">
-      <c r="A161" s="2" t="inlineStr">
+      <c r="A161" s="3" t="inlineStr">
         <is>
           <t>RUG766</t>
         </is>
@@ -52546,9 +53370,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J161" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="162">
-      <c r="A162" s="2" t="inlineStr">
+      <c r="A162" s="3" t="inlineStr">
         <is>
           <t>RUG059</t>
         </is>
@@ -52581,9 +53410,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J162" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="163">
-      <c r="A163" s="2" t="inlineStr">
+      <c r="A163" s="3" t="inlineStr">
         <is>
           <t>RUG358</t>
         </is>
@@ -52616,9 +53450,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J163" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="164">
-      <c r="A164" s="2" t="inlineStr">
+      <c r="A164" s="3" t="inlineStr">
         <is>
           <t>RUG753</t>
         </is>
@@ -52651,9 +53490,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J164" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="165">
-      <c r="A165" s="2" t="inlineStr">
+      <c r="A165" s="3" t="inlineStr">
         <is>
           <t>RUG348</t>
         </is>
@@ -52686,9 +53530,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J165" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="166">
-      <c r="A166" s="2" t="inlineStr">
+      <c r="A166" s="3" t="inlineStr">
         <is>
           <t>RUG312</t>
         </is>
@@ -52721,9 +53570,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J166" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="167">
-      <c r="A167" s="2" t="inlineStr">
+      <c r="A167" s="3" t="inlineStr">
         <is>
           <t>RUG071</t>
         </is>
@@ -52756,9 +53610,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J167" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="168">
-      <c r="A168" s="2" t="inlineStr">
+      <c r="A168" s="3" t="inlineStr">
         <is>
           <t>RUG620</t>
         </is>
@@ -52791,9 +53650,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J168" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="169">
-      <c r="A169" s="2" t="inlineStr">
+      <c r="A169" s="3" t="inlineStr">
         <is>
           <t>RUG265</t>
         </is>
@@ -52826,9 +53690,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J169" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="170">
-      <c r="A170" s="2" t="inlineStr">
+      <c r="A170" s="3" t="inlineStr">
         <is>
           <t>RUG785</t>
         </is>
@@ -52861,9 +53730,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J170" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="171">
-      <c r="A171" s="2" t="inlineStr">
+      <c r="A171" s="3" t="inlineStr">
         <is>
           <t>RUG249</t>
         </is>
@@ -52896,9 +53770,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J171" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="172">
-      <c r="A172" s="2" t="inlineStr">
+      <c r="A172" s="3" t="inlineStr">
         <is>
           <t>RUG668</t>
         </is>
@@ -52931,9 +53810,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J172" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="173">
-      <c r="A173" s="2" t="inlineStr">
+      <c r="A173" s="3" t="inlineStr">
         <is>
           <t>RUG430</t>
         </is>
@@ -52966,9 +53850,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J173" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="174">
-      <c r="A174" s="2" t="inlineStr">
+      <c r="A174" s="3" t="inlineStr">
         <is>
           <t>RUG424</t>
         </is>
@@ -53001,9 +53890,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J174" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="175">
-      <c r="A175" s="2" t="inlineStr">
+      <c r="A175" s="3" t="inlineStr">
         <is>
           <t>RUG224</t>
         </is>
@@ -53036,9 +53930,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J175" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="176">
-      <c r="A176" s="2" t="inlineStr">
+      <c r="A176" s="3" t="inlineStr">
         <is>
           <t>RUG443</t>
         </is>
@@ -53071,9 +53970,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J176" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="177">
-      <c r="A177" s="2" t="inlineStr">
+      <c r="A177" s="3" t="inlineStr">
         <is>
           <t>RUG134</t>
         </is>
@@ -53106,9 +54010,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J177" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="178">
-      <c r="A178" s="2" t="inlineStr">
+      <c r="A178" s="3" t="inlineStr">
         <is>
           <t>RUG228</t>
         </is>
@@ -53141,9 +54050,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J178" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="179">
-      <c r="A179" s="2" t="inlineStr">
+      <c r="A179" s="3" t="inlineStr">
         <is>
           <t>RUG136</t>
         </is>
@@ -53176,9 +54090,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J179" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="180">
-      <c r="A180" s="2" t="inlineStr">
+      <c r="A180" s="3" t="inlineStr">
         <is>
           <t>RUG599</t>
         </is>
@@ -53211,9 +54130,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J180" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="181">
-      <c r="A181" s="2" t="inlineStr">
+      <c r="A181" s="3" t="inlineStr">
         <is>
           <t>hRUG913</t>
         </is>
@@ -53246,9 +54170,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J181" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="182">
-      <c r="A182" s="2" t="inlineStr">
+      <c r="A182" s="3" t="inlineStr">
         <is>
           <t>RUG496</t>
         </is>
@@ -53281,9 +54210,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J182" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="183">
-      <c r="A183" s="2" t="inlineStr">
+      <c r="A183" s="3" t="inlineStr">
         <is>
           <t>RUG204</t>
         </is>
@@ -53316,9 +54250,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J183" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="184">
-      <c r="A184" s="2" t="inlineStr">
+      <c r="A184" s="3" t="inlineStr">
         <is>
           <t>RUG533</t>
         </is>
@@ -53351,9 +54290,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J184" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="185">
-      <c r="A185" s="2" t="inlineStr">
+      <c r="A185" s="3" t="inlineStr">
         <is>
           <t>RUG182</t>
         </is>
@@ -53386,9 +54330,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J185" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="186">
-      <c r="A186" s="2" t="inlineStr">
+      <c r="A186" s="3" t="inlineStr">
         <is>
           <t>RUG413</t>
         </is>
@@ -53421,9 +54370,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J186" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="187">
-      <c r="A187" s="2" t="inlineStr">
+      <c r="A187" s="3" t="inlineStr">
         <is>
           <t>RUG839</t>
         </is>
@@ -53456,9 +54410,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J187" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="188">
-      <c r="A188" s="2" t="inlineStr">
+      <c r="A188" s="3" t="inlineStr">
         <is>
           <t>RUG403</t>
         </is>
@@ -53491,9 +54450,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J188" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="189">
-      <c r="A189" s="2" t="inlineStr">
+      <c r="A189" s="3" t="inlineStr">
         <is>
           <t>RUG137</t>
         </is>
@@ -53526,9 +54490,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J189" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="190">
-      <c r="A190" s="2" t="inlineStr">
+      <c r="A190" s="3" t="inlineStr">
         <is>
           <t>RUG415</t>
         </is>
@@ -53561,9 +54530,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J190" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="191">
-      <c r="A191" s="2" t="inlineStr">
+      <c r="A191" s="3" t="inlineStr">
         <is>
           <t>RUG571</t>
         </is>
@@ -53596,9 +54570,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J191" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="192">
-      <c r="A192" s="2" t="inlineStr">
+      <c r="A192" s="3" t="inlineStr">
         <is>
           <t>RUG317</t>
         </is>
@@ -53631,9 +54610,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J192" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="193">
-      <c r="A193" s="2" t="inlineStr">
+      <c r="A193" s="3" t="inlineStr">
         <is>
           <t>RUG815</t>
         </is>
@@ -53666,9 +54650,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J193" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="194">
-      <c r="A194" s="2" t="inlineStr">
+      <c r="A194" s="3" t="inlineStr">
         <is>
           <t>RUG069</t>
         </is>
@@ -53701,9 +54690,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J194" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="195">
-      <c r="A195" s="2" t="inlineStr">
+      <c r="A195" s="3" t="inlineStr">
         <is>
           <t>RUG073</t>
         </is>
@@ -53736,9 +54730,14 @@
           <t>c__Bacteroidia</t>
         </is>
       </c>
+      <c r="J195" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
     </row>
     <row r="196">
-      <c r="A196" s="2" t="inlineStr">
+      <c r="A196" s="3" t="inlineStr">
         <is>
           <t>RUG544</t>
         </is>
@@ -53767,6 +54766,11 @@
         </is>
       </c>
       <c r="I196" t="inlineStr">
+        <is>
+          <t>c__Bacteroidia</t>
+        </is>
+      </c>
+      <c r="J196" t="inlineStr">
         <is>
           <t>c__Bacteroidia</t>
         </is>
@@ -61441,7 +62445,7 @@
   </sheetPr>
   <dimension ref="A1:I128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>